<commit_message>
updating with desktopOnly checks for mobile
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\_dev\puppeteer-screenshots-testing\puppeteer-screenshots-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB62F72-F8B4-41FE-AC83-F1B826B18B80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161B8AE8-8F04-49FC-9F9F-19774EF11E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D8F16D84-C719-496E-9A19-56A036201834}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Home</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Landing</t>
+  </si>
+  <si>
+    <t>desktopOnly</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C7ACE2-88C4-4F99-9808-7430D2D41EE9}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -454,9 +457,10 @@
     <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.46484375" customWidth="1"/>
     <col min="4" max="4" width="19.73046875" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -469,8 +473,11 @@
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -484,7 +491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -493,6 +500,9 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>